<commit_message>
updated descriptions of tests per requirements.
</commit_message>
<xml_diff>
--- a/ClueLayoutPart3.xlsx
+++ b/ClueLayoutPart3.xlsx
@@ -104,9 +104,6 @@
     <t>locations within rooms (1)</t>
   </si>
   <si>
-    <t>at the edge of the board (4)</t>
-  </si>
-  <si>
     <t>beside a room that is not a doorway (2)</t>
   </si>
   <si>
@@ -129,6 +126,9 @@
   </si>
   <si>
     <t>Adjacency Tests</t>
+  </si>
+  <si>
+    <t>at the edge of the board (4) (assuming corners count as edges)</t>
   </si>
 </sst>
 </file>
@@ -293,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -311,11 +311,22 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -333,18 +344,8 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -632,8 +633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -968,7 +969,7 @@
       <c r="R5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="S5" s="8" t="s">
+      <c r="S5" s="12" t="s">
         <v>10</v>
       </c>
       <c r="T5" s="6" t="s">
@@ -1009,7 +1010,7 @@
       <c r="I6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="17" t="s">
+      <c r="J6" s="28" t="s">
         <v>10</v>
       </c>
       <c r="K6" s="8" t="s">
@@ -1062,7 +1063,7 @@
       <c r="D7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="8" t="s">
         <v>10</v>
       </c>
       <c r="F7" s="8" t="s">
@@ -1299,7 +1300,7 @@
       <c r="O10" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="P10" s="17" t="s">
+      <c r="P10" s="28" t="s">
         <v>10</v>
       </c>
       <c r="Q10" s="8" t="s">
@@ -1340,7 +1341,7 @@
       <c r="F11" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="17" t="s">
+      <c r="G11" s="28" t="s">
         <v>10</v>
       </c>
       <c r="H11" s="4" t="s">
@@ -1600,7 +1601,7 @@
       <c r="B15" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D15" s="8" t="s">
@@ -1645,7 +1646,7 @@
       <c r="Q15" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="R15" s="8" t="s">
+      <c r="R15" s="28" t="s">
         <v>10</v>
       </c>
       <c r="S15" s="8" t="s">
@@ -1677,7 +1678,7 @@
       <c r="E16" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="F16" s="8" t="s">
         <v>10</v>
       </c>
       <c r="G16" s="8" t="s">
@@ -1751,7 +1752,7 @@
       <c r="G17" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H17" s="17" t="s">
+      <c r="H17" s="8" t="s">
         <v>10</v>
       </c>
       <c r="I17" s="7" t="s">
@@ -2047,7 +2048,7 @@
       <c r="O21" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="P21" s="8" t="s">
+      <c r="P21" s="28" t="s">
         <v>10</v>
       </c>
       <c r="Q21" s="7" t="s">
@@ -2205,128 +2206,136 @@
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A26" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A27" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="23"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A28" s="24" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A26" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19"/>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A27" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="B27" s="20"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19"/>
-    </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A28" s="21" t="s">
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="17"/>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A29" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-    </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A29" s="22" t="s">
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="17"/>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A30" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="22"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="22"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-    </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A30" s="23" t="s">
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="L30" s="29"/>
+      <c r="M30" s="29"/>
+      <c r="N30" s="29"/>
+      <c r="O30" s="29"/>
+      <c r="P30" s="29"/>
+      <c r="Q30" s="29"/>
+      <c r="R30" s="29"/>
+      <c r="S30" s="29"/>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A31" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="23"/>
-      <c r="C30" s="23"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="23"/>
-    </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A31" s="24" t="s">
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="17"/>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A32" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" s="17"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="17"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="24"/>
-      <c r="C31" s="24"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="19"/>
-    </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A32" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="B32" s="19"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="19"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="26" t="s">
+      <c r="B33" s="19"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="17"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="26"/>
-      <c r="C33" s="26"/>
-      <c r="D33" s="26"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="19"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="27" t="s">
+      <c r="B34" s="20"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="17"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="B34" s="27"/>
-      <c r="C34" s="27"/>
-      <c r="D34" s="27"/>
-      <c r="E34" s="27"/>
-      <c r="F34" s="27"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="19"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="B35" s="28"/>
-      <c r="C35" s="28"/>
-      <c r="D35" s="28"/>
-      <c r="E35" s="28"/>
-      <c r="F35" s="28"/>
-      <c r="G35" s="19"/>
-      <c r="H35" s="19"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>